<commit_message>
Fixed P3HT Hansen Param
</commit_message>
<xml_diff>
--- a/Functions/Solvs.xlsx
+++ b/Functions/Solvs.xlsx
@@ -442,7 +442,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -455,7 +455,7 @@
         <v>19.45</v>
       </c>
       <c r="C1">
-        <v>3.17</v>
+        <v>3.97</v>
       </c>
       <c r="D1">
         <v>4.1900000000000004</v>

</xml_diff>